<commit_message>
Update for variable log file
</commit_message>
<xml_diff>
--- a/data/log_data_postprocess.xlsx
+++ b/data/log_data_postprocess.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProject\EDA-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A040422F-3AFF-4A29-8189-6757374A5AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A4CCC1-F895-45EF-8D29-EE922C1C4ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B16BB66F-007C-416B-8A77-4B4F8B6782B4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="222">
   <si>
     <t>corrected_variable_name</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>cat_hus_dir_fce</t>
-  </si>
-  <si>
-    <t>Not yet</t>
   </si>
   <si>
     <t>Direction of facing of a house</t>
@@ -866,7 +863,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,6 +895,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1036,7 +1039,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1071,28 +1074,46 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1113,9 +1134,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1128,12 +1146,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1143,35 +1155,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1490,9 +1496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA5C2C4-4AF8-44A6-8680-53141E329A99}">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G71" sqref="G71:G79"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,20 +1513,20 @@
     <col min="9" max="9" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="82.85546875" style="36" customWidth="1"/>
+    <col min="12" max="12" width="82.85546875" style="15" customWidth="1"/>
     <col min="13" max="15" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -1550,35 +1556,35 @@
         <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>195</v>
-      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="24">
         <v>3</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="24" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="5">
@@ -1593,27 +1599,27 @@
       <c r="K2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>196</v>
+      <c r="L2" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="3">
         <v>21</v>
       </c>
@@ -1626,19 +1632,19 @@
       <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="3">
         <v>22</v>
       </c>
@@ -1651,19 +1657,19 @@
       <c r="K4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="5">
         <v>23</v>
       </c>
@@ -1676,19 +1682,19 @@
       <c r="K5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="3">
         <v>24</v>
       </c>
@@ -1701,19 +1707,19 @@
       <c r="K6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="6">
         <v>25</v>
       </c>
@@ -1726,19 +1732,19 @@
       <c r="K7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="3">
         <v>26</v>
       </c>
@@ -1751,19 +1757,19 @@
       <c r="K8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="6">
         <v>29</v>
       </c>
@@ -1776,19 +1782,19 @@
       <c r="K9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="28"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="5">
         <v>31</v>
       </c>
@@ -1801,19 +1807,19 @@
       <c r="K10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="28"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="5">
         <v>32</v>
       </c>
@@ -1826,19 +1832,19 @@
       <c r="K11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="28"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="6">
         <v>33</v>
       </c>
@@ -1851,19 +1857,19 @@
       <c r="K12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="28"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="6">
         <v>34</v>
       </c>
@@ -1876,19 +1882,19 @@
       <c r="K13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="28"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="3">
         <v>35</v>
       </c>
@@ -1901,19 +1907,19 @@
       <c r="K14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="28"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="3">
         <v>36</v>
       </c>
@@ -1926,19 +1932,19 @@
       <c r="K15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="28"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="6">
         <v>37</v>
       </c>
@@ -1951,19 +1957,19 @@
       <c r="K16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="28"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="3">
         <v>38</v>
       </c>
@@ -1976,19 +1982,19 @@
       <c r="K17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="28"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="3">
         <v>39</v>
       </c>
@@ -2001,31 +2007,31 @@
       <c r="K18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="28"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="D19" s="14" t="s">
+      <c r="B19" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="22">
         <v>2</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="4">
@@ -2040,27 +2046,27 @@
       <c r="K19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L19" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="N19" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="O19" s="13" t="s">
-        <v>196</v>
+      <c r="L19" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="O19" s="21" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="4">
         <v>2</v>
       </c>
@@ -2073,19 +2079,19 @@
       <c r="K20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L20" s="30"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="4">
         <v>3</v>
       </c>
@@ -2098,31 +2104,31 @@
       <c r="K21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="30"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="B22" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="24">
         <v>3</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="24" t="s">
         <v>41</v>
       </c>
       <c r="H22" s="3">
@@ -2133,27 +2139,27 @@
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="O22" s="12" t="s">
-        <v>196</v>
+      <c r="L22" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="M22" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="N22" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="O22" s="24" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="3">
         <v>2</v>
       </c>
@@ -2162,19 +2168,19 @@
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="3">
         <v>3</v>
       </c>
@@ -2183,20 +2189,20 @@
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>49</v>
@@ -2212,17 +2218,17 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="31" t="s">
-        <v>201</v>
+      <c r="L25" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2230,10 +2236,10 @@
         <v>48</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>50</v>
@@ -2249,1575 +2255,1583 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="32" t="s">
-        <v>217</v>
+      <c r="L26" s="14" t="s">
+        <v>216</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="D27" s="14" t="s">
+      <c r="B27" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="22">
+        <v>4</v>
+      </c>
+      <c r="G27" s="22" t="s">
         <v>56</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H27" s="11">
         <v>1</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J27" s="11">
         <v>3</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="L27" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="M27" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="N27" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="O27" s="13" t="s">
-        <v>196</v>
+        <v>57</v>
+      </c>
+      <c r="L27" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="M27" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="O27" s="21" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
       <c r="H28" s="11">
         <v>2</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J28" s="11">
         <v>3</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="L28" s="30"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
+        <v>58</v>
+      </c>
+      <c r="L28" s="35"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="4">
         <v>3</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J29" s="4">
         <v>1</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L29" s="30"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="L29" s="35"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
       <c r="H30" s="5">
         <v>4</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J30" s="5">
         <v>4</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L30" s="30"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
+        <v>60</v>
+      </c>
+      <c r="L30" s="35"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
       <c r="H31" s="6">
         <v>5</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J31" s="6">
         <v>2</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L31" s="30"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
+        <v>61</v>
+      </c>
+      <c r="L31" s="35"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
       <c r="H32" s="6">
         <v>6</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J32" s="6">
         <v>2</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="L32" s="30"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
+        <v>62</v>
+      </c>
+      <c r="L32" s="35"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
       <c r="H33" s="5">
         <v>7</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J33" s="5">
         <v>4</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L33" s="30"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
+        <v>63</v>
+      </c>
+      <c r="L33" s="35"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="5">
         <v>8</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J34" s="5">
         <v>4</v>
       </c>
       <c r="K34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" s="35"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="L34" s="30"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+      <c r="B35" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26" t="s">
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E36" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26" t="s">
+      <c r="F36" s="12"/>
+      <c r="G36" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="M36" s="43"/>
-      <c r="N36" s="43"/>
-      <c r="O36" s="43"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="D37" s="20" t="s">
+      <c r="A37" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="26">
+        <v>6</v>
+      </c>
+      <c r="G37" s="26" t="s">
         <v>183</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20" t="s">
-        <v>184</v>
       </c>
       <c r="H37" s="8">
         <v>1</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
-      <c r="L37" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="M37" s="20" t="s">
+      <c r="L37" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="N37" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="O37" s="20" t="s">
-        <v>196</v>
+      <c r="M37" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="N37" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="O37" s="26" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="8">
         <v>2</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
-      <c r="O38" s="21"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="8">
         <v>3</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
       <c r="H40" s="8">
         <v>4</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
       <c r="H41" s="8">
         <v>5</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="34"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
       <c r="H42" s="8">
         <v>6</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="32" t="s">
-        <v>208</v>
+      <c r="L43" s="14" t="s">
+        <v>207</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O43" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="31" t="s">
-        <v>202</v>
+      <c r="L44" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O44" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D45" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="C45" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" s="44" t="s">
+      <c r="E45" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E45" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="M45" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="N45" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="O45" s="44" t="s">
-        <v>196</v>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="M45" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="N45" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="O45" s="19" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="31" t="s">
-        <v>219</v>
+      <c r="L46" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O46" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
-      <c r="L47" s="32" t="s">
+      <c r="L47" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="N47" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="O47" s="7"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="M47" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="N47" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="O47" s="7"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+      <c r="B48" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="D48" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="D48" s="14" t="s">
+      <c r="E48" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="22">
+        <v>5</v>
+      </c>
+      <c r="G48" s="22" t="s">
         <v>88</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>89</v>
       </c>
       <c r="H48" s="11">
         <v>1</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J48" s="11">
         <v>5</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="L48" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="M48" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="N48" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="O48" s="13" t="s">
-        <v>196</v>
+        <v>89</v>
+      </c>
+      <c r="L48" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="M48" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="N48" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="O48" s="21" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
       <c r="H49" s="10">
         <v>2</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J49" s="10">
         <v>2</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="L49" s="30"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
+        <v>90</v>
+      </c>
+      <c r="L49" s="35"/>
+      <c r="M49" s="22"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="22"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
       <c r="H50" s="10">
         <v>3</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J50" s="10">
         <v>2</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="L50" s="30"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
+        <v>91</v>
+      </c>
+      <c r="L50" s="35"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
       <c r="H51" s="9">
         <v>4</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J51" s="9">
         <v>1</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="L51" s="30"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
+        <v>92</v>
+      </c>
+      <c r="L51" s="35"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
       <c r="H52" s="9">
         <v>5</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J52" s="9">
         <v>1</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="L52" s="30"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
+        <v>93</v>
+      </c>
+      <c r="L52" s="35"/>
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
       <c r="H53" s="4">
         <v>6</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J53" s="4">
         <v>3</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="L53" s="30"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
+        <v>94</v>
+      </c>
+      <c r="L53" s="35"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="22"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
       <c r="H54" s="5">
         <v>7</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J54" s="5">
         <v>4</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="L54" s="30"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
+        <v>95</v>
+      </c>
+      <c r="L54" s="35"/>
+      <c r="M54" s="22"/>
+      <c r="N54" s="22"/>
+      <c r="O54" s="22"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
       <c r="H55" s="5">
         <v>8</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J55" s="5">
         <v>4</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L55" s="30"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
+        <v>96</v>
+      </c>
+      <c r="L55" s="35"/>
+      <c r="M55" s="22"/>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
+      <c r="A56" s="22"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
       <c r="H56" s="11">
         <v>9</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J56" s="11">
         <v>5</v>
       </c>
       <c r="K56" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="L56" s="35"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="L56" s="30"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
-      <c r="O56" s="14"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+      <c r="B57" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="D57" s="12" t="s">
+      <c r="E57" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="24">
+        <v>3</v>
+      </c>
+      <c r="G57" s="24" t="s">
         <v>100</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="H57" s="3">
         <v>1</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
-      <c r="L57" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="M57" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="N57" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="O57" s="15" t="s">
-        <v>196</v>
+      <c r="L57" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="M57" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="N57" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="O57" s="23" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
       <c r="H58" s="3">
         <v>2</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="28"/>
-      <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
-      <c r="O58" s="12"/>
+      <c r="L58" s="33"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
+      <c r="O58" s="24"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
+      <c r="A59" s="24"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
       <c r="H59" s="3">
         <v>3</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
-      <c r="L59" s="28"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="12"/>
-      <c r="O59" s="12"/>
+      <c r="L59" s="33"/>
+      <c r="M59" s="24"/>
+      <c r="N59" s="24"/>
+      <c r="O59" s="24"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="3">
+      <c r="A60" s="24"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="40">
         <v>4</v>
       </c>
-      <c r="I60" s="3" t="s">
-        <v>105</v>
+      <c r="I60" s="40" t="s">
+        <v>104</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
-      <c r="L60" s="28"/>
-      <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="12"/>
+      <c r="L60" s="33"/>
+      <c r="M60" s="24"/>
+      <c r="N60" s="24"/>
+      <c r="O60" s="24"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="3">
+      <c r="A61" s="24"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="40">
         <v>5</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>106</v>
+      <c r="I61" s="40" t="s">
+        <v>105</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="12"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="12"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="24"/>
+      <c r="N61" s="24"/>
+      <c r="O61" s="24"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="C62" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="D62" s="14" t="s">
+      <c r="E62" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="22">
+        <v>3</v>
+      </c>
+      <c r="G62" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E62" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="H62" s="4">
+      <c r="H62" s="40">
         <v>1</v>
       </c>
-      <c r="I62" s="4" t="s">
-        <v>90</v>
+      <c r="I62" s="40" t="s">
+        <v>89</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="M62" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="N62" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="O62" s="13" t="s">
-        <v>196</v>
+      <c r="L62" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="M62" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="N62" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="O62" s="21" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="4">
+      <c r="A63" s="22"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="40">
         <v>2</v>
       </c>
-      <c r="I63" s="4" t="s">
-        <v>110</v>
+      <c r="I63" s="40" t="s">
+        <v>109</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
-      <c r="L63" s="30"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="14"/>
-      <c r="O63" s="14"/>
+      <c r="L63" s="35"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="22"/>
+      <c r="O63" s="22"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
       <c r="H64" s="4">
         <v>3</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="30"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="14"/>
-      <c r="O64" s="14"/>
+      <c r="L64" s="35"/>
+      <c r="M64" s="22"/>
+      <c r="N64" s="22"/>
+      <c r="O64" s="22"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
+      <c r="A65" s="22"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
       <c r="H65" s="4">
         <v>4</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
-      <c r="L65" s="30"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-      <c r="O65" s="14"/>
+      <c r="L65" s="35"/>
+      <c r="M65" s="22"/>
+      <c r="N65" s="22"/>
+      <c r="O65" s="22"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
+      <c r="A66" s="22"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
       <c r="H66" s="4">
         <v>5</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
-      <c r="L66" s="30"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14"/>
-      <c r="O66" s="14"/>
+      <c r="L66" s="35"/>
+      <c r="M66" s="22"/>
+      <c r="N66" s="22"/>
+      <c r="O66" s="22"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="4">
+      <c r="A67" s="22"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="40">
         <v>6</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="I67" s="40" t="s">
         <v>37</v>
       </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="30"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
-      <c r="O67" s="14"/>
+      <c r="L67" s="35"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="22"/>
+      <c r="O67" s="22"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="38" t="s">
+      <c r="A68" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="C68" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="D68" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B68" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="C68" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="D68" s="38" t="s">
+      <c r="E68" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F68" s="41">
+        <v>2</v>
+      </c>
+      <c r="G68" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H68" s="40">
+        <v>1</v>
+      </c>
+      <c r="I68" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="E68" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F68" s="38">
+      <c r="J68" s="16"/>
+      <c r="K68" s="16"/>
+      <c r="L68" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="M68" s="25"/>
+      <c r="N68" s="25"/>
+      <c r="O68" s="25"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="42"/>
+      <c r="B69" s="42"/>
+      <c r="C69" s="42"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
+      <c r="H69" s="40">
         <v>2</v>
       </c>
-      <c r="G68" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="H68" s="37">
-        <v>1</v>
-      </c>
-      <c r="I68" s="37" t="s">
+      <c r="I69" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="J68" s="37"/>
-      <c r="K68" s="37"/>
-      <c r="L68" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="M68" s="38"/>
-      <c r="N68" s="38"/>
-      <c r="O68" s="38"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="38"/>
-      <c r="B69" s="41"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="37">
-        <v>2</v>
-      </c>
-      <c r="I69" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="J69" s="37"/>
-      <c r="K69" s="37"/>
-      <c r="L69" s="40"/>
-      <c r="M69" s="38"/>
-      <c r="N69" s="38"/>
-      <c r="O69" s="38"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="16"/>
+      <c r="L69" s="39"/>
+      <c r="M69" s="25"/>
+      <c r="N69" s="25"/>
+      <c r="O69" s="25"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="31" t="s">
-        <v>222</v>
+      <c r="L70" s="13" t="s">
+        <v>221</v>
       </c>
       <c r="M70" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N70" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="O70" s="8"/>
+        <v>195</v>
+      </c>
+      <c r="O70" s="8" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B71" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="B71" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="C71" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="D71" s="12" t="s">
+      <c r="E71" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F71" s="24">
+        <v>3</v>
+      </c>
+      <c r="G71" s="24" t="s">
         <v>121</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F71" s="12">
-        <v>3</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>122</v>
       </c>
       <c r="H71" s="3">
         <v>1</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J71" s="3">
         <v>1</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="L71" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="M71" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="N71" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="O71" s="15"/>
+        <v>122</v>
+      </c>
+      <c r="L71" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="M71" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="N71" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="O71" s="23" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="16"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
       <c r="H72" s="3">
         <v>2</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J72" s="3">
         <v>1</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="L72" s="28"/>
-      <c r="M72" s="12"/>
-      <c r="N72" s="12"/>
-      <c r="O72" s="12"/>
+        <v>123</v>
+      </c>
+      <c r="L72" s="33"/>
+      <c r="M72" s="24"/>
+      <c r="N72" s="24"/>
+      <c r="O72" s="24"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
       <c r="H73" s="3">
         <v>3</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J73" s="3">
         <v>1</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="L73" s="28"/>
-      <c r="M73" s="12"/>
-      <c r="N73" s="12"/>
-      <c r="O73" s="12"/>
+        <v>124</v>
+      </c>
+      <c r="L73" s="33"/>
+      <c r="M73" s="24"/>
+      <c r="N73" s="24"/>
+      <c r="O73" s="24"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
+      <c r="A74" s="43"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
       <c r="H74" s="3">
         <v>4</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J74" s="3">
         <v>2</v>
       </c>
       <c r="K74" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L74" s="28"/>
-      <c r="M74" s="12"/>
-      <c r="N74" s="12"/>
-      <c r="O74" s="12"/>
+        <v>125</v>
+      </c>
+      <c r="L74" s="33"/>
+      <c r="M74" s="24"/>
+      <c r="N74" s="24"/>
+      <c r="O74" s="24"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
       <c r="H75" s="3">
         <v>5</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J75" s="3">
         <v>2</v>
       </c>
       <c r="K75" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="L75" s="28"/>
-      <c r="M75" s="12"/>
-      <c r="N75" s="12"/>
-      <c r="O75" s="12"/>
+        <v>126</v>
+      </c>
+      <c r="L75" s="33"/>
+      <c r="M75" s="24"/>
+      <c r="N75" s="24"/>
+      <c r="O75" s="24"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" s="16"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
       <c r="H76" s="3">
         <v>6</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J76" s="3">
         <v>2</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="L76" s="28"/>
-      <c r="M76" s="12"/>
-      <c r="N76" s="12"/>
-      <c r="O76" s="12"/>
+        <v>127</v>
+      </c>
+      <c r="L76" s="33"/>
+      <c r="M76" s="24"/>
+      <c r="N76" s="24"/>
+      <c r="O76" s="24"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" s="16"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="43"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
       <c r="H77" s="3">
         <v>7</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J77" s="3">
         <v>2</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="L77" s="28"/>
-      <c r="M77" s="12"/>
-      <c r="N77" s="12"/>
-      <c r="O77" s="12"/>
+        <v>128</v>
+      </c>
+      <c r="L77" s="33"/>
+      <c r="M77" s="24"/>
+      <c r="N77" s="24"/>
+      <c r="O77" s="24"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78" s="16"/>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
       <c r="H78" s="3">
         <v>8</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J78" s="3">
         <v>3</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="L78" s="28"/>
-      <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
-      <c r="O78" s="12"/>
+        <v>129</v>
+      </c>
+      <c r="L78" s="33"/>
+      <c r="M78" s="24"/>
+      <c r="N78" s="24"/>
+      <c r="O78" s="24"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
+      <c r="A79" s="43"/>
+      <c r="B79" s="43"/>
+      <c r="C79" s="43"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
       <c r="H79" s="3">
         <v>9</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J79" s="3">
         <v>3</v>
       </c>
       <c r="K79" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="L79" s="33"/>
+      <c r="M79" s="24"/>
+      <c r="N79" s="24"/>
+      <c r="O79" s="24"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L79" s="28"/>
-      <c r="M79" s="12"/>
-      <c r="N79" s="12"/>
-      <c r="O79" s="12"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+      <c r="B80" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D80" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="C80" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="D80" s="14" t="s">
+      <c r="E80" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F80" s="22">
+        <v>4</v>
+      </c>
+      <c r="G80" s="22" t="s">
         <v>133</v>
-      </c>
-      <c r="E80" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F80" s="14">
-        <v>4</v>
-      </c>
-      <c r="G80" s="14" t="s">
-        <v>134</v>
       </c>
       <c r="H80" s="4">
         <v>1</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
-      <c r="L80" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="M80" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="N80" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="O80" s="13"/>
+      <c r="L80" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M80" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="N80" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="O80" s="21" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
       <c r="H81" s="4">
         <v>2</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
-      <c r="L81" s="30"/>
-      <c r="M81" s="14"/>
-      <c r="N81" s="14"/>
-      <c r="O81" s="14"/>
+      <c r="L81" s="35"/>
+      <c r="M81" s="22"/>
+      <c r="N81" s="22"/>
+      <c r="O81" s="22"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
       <c r="H82" s="4">
         <v>3</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
-      <c r="L82" s="30"/>
-      <c r="M82" s="14"/>
-      <c r="N82" s="14"/>
-      <c r="O82" s="14"/>
+      <c r="L82" s="35"/>
+      <c r="M82" s="22"/>
+      <c r="N82" s="22"/>
+      <c r="O82" s="22"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
+      <c r="A83" s="22"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
       <c r="H83" s="4">
         <v>4</v>
       </c>
@@ -3826,322 +3840,414 @@
       </c>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
-      <c r="L83" s="30"/>
-      <c r="M83" s="14"/>
-      <c r="N83" s="14"/>
-      <c r="O83" s="14"/>
+      <c r="L83" s="35"/>
+      <c r="M83" s="22"/>
+      <c r="N83" s="22"/>
+      <c r="O83" s="22"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
+      <c r="A84" s="22"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
       <c r="H84" s="4">
         <v>5</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
-      <c r="L84" s="30"/>
-      <c r="M84" s="14"/>
-      <c r="N84" s="14"/>
-      <c r="O84" s="14"/>
+      <c r="L84" s="35"/>
+      <c r="M84" s="22"/>
+      <c r="N84" s="22"/>
+      <c r="O84" s="22"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B85" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="D85" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="B85" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="D85" s="12" t="s">
+      <c r="E85" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F85" s="24">
+        <v>7</v>
+      </c>
+      <c r="G85" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F85" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G85" s="12" t="s">
-        <v>141</v>
       </c>
       <c r="H85" s="3">
         <v>1</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J85" s="3">
         <v>1</v>
       </c>
       <c r="K85" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="L85" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="M85" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="N85" s="15"/>
-      <c r="O85" s="15"/>
+        <v>141</v>
+      </c>
+      <c r="L85" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="M85" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="N85" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="O85" s="23" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
+      <c r="A86" s="24"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
       <c r="H86" s="3">
         <v>2</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J86" s="3">
         <v>2</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="L86" s="28"/>
-      <c r="M86" s="12"/>
-      <c r="N86" s="12"/>
-      <c r="O86" s="12"/>
+        <v>142</v>
+      </c>
+      <c r="L86" s="33"/>
+      <c r="M86" s="24"/>
+      <c r="N86" s="24"/>
+      <c r="O86" s="24"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
+      <c r="A87" s="24"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
       <c r="H87" s="3">
         <v>3</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J87" s="3">
         <v>3</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="L87" s="28"/>
-      <c r="M87" s="12"/>
-      <c r="N87" s="12"/>
-      <c r="O87" s="12"/>
+        <v>143</v>
+      </c>
+      <c r="L87" s="33"/>
+      <c r="M87" s="24"/>
+      <c r="N87" s="24"/>
+      <c r="O87" s="24"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
+      <c r="A88" s="24"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
       <c r="H88" s="3">
         <v>4</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J88" s="3">
         <v>4</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="L88" s="28"/>
-      <c r="M88" s="12"/>
-      <c r="N88" s="12"/>
-      <c r="O88" s="12"/>
+        <v>144</v>
+      </c>
+      <c r="L88" s="33"/>
+      <c r="M88" s="24"/>
+      <c r="N88" s="24"/>
+      <c r="O88" s="24"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
-      <c r="G89" s="12"/>
+      <c r="A89" s="24"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
       <c r="H89" s="3">
         <v>5</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J89" s="3">
         <v>5</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L89" s="28"/>
-      <c r="M89" s="12"/>
-      <c r="N89" s="12"/>
-      <c r="O89" s="12"/>
+        <v>145</v>
+      </c>
+      <c r="L89" s="33"/>
+      <c r="M89" s="24"/>
+      <c r="N89" s="24"/>
+      <c r="O89" s="24"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
+      <c r="A90" s="24"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
       <c r="H90" s="3">
         <v>6</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J90" s="3">
         <v>6</v>
       </c>
       <c r="K90" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="L90" s="28"/>
-      <c r="M90" s="12"/>
-      <c r="N90" s="12"/>
-      <c r="O90" s="12"/>
+        <v>146</v>
+      </c>
+      <c r="L90" s="33"/>
+      <c r="M90" s="24"/>
+      <c r="N90" s="24"/>
+      <c r="O90" s="24"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
-      <c r="C91" s="12"/>
-      <c r="D91" s="12"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="12"/>
+      <c r="A91" s="24"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
       <c r="H91" s="3">
         <v>7</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J91" s="3">
         <v>7</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="L91" s="28"/>
-      <c r="M91" s="12"/>
-      <c r="N91" s="12"/>
-      <c r="O91" s="12"/>
+        <v>147</v>
+      </c>
+      <c r="L91" s="33"/>
+      <c r="M91" s="24"/>
+      <c r="N91" s="24"/>
+      <c r="O91" s="24"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="12"/>
-      <c r="D92" s="12"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
+      <c r="A92" s="24"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
       <c r="H92" s="3">
         <v>8</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J92" s="3">
         <v>7</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="L92" s="28"/>
-      <c r="M92" s="12"/>
-      <c r="N92" s="12"/>
-      <c r="O92" s="12"/>
+        <v>148</v>
+      </c>
+      <c r="L92" s="33"/>
+      <c r="M92" s="24"/>
+      <c r="N92" s="24"/>
+      <c r="O92" s="24"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
+      <c r="A93" s="24"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
       <c r="H93" s="3">
         <v>9</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J93" s="3">
         <v>7</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="L93" s="28"/>
-      <c r="M93" s="12"/>
-      <c r="N93" s="12"/>
-      <c r="O93" s="12"/>
+        <v>149</v>
+      </c>
+      <c r="L93" s="33"/>
+      <c r="M93" s="24"/>
+      <c r="N93" s="24"/>
+      <c r="O93" s="24"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
-      <c r="L94" s="31" t="s">
-        <v>154</v>
+      <c r="L94" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="M94" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="N94" s="8"/>
-      <c r="O94" s="8"/>
+        <v>195</v>
+      </c>
+      <c r="N94" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="O94" s="8" t="s">
+        <v>195</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="132">
-    <mergeCell ref="O80:O84"/>
-    <mergeCell ref="O85:O93"/>
-    <mergeCell ref="O48:O56"/>
-    <mergeCell ref="O57:O61"/>
-    <mergeCell ref="O62:O67"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="O71:O79"/>
-    <mergeCell ref="O2:O18"/>
-    <mergeCell ref="O19:O21"/>
-    <mergeCell ref="O22:O24"/>
-    <mergeCell ref="O27:O34"/>
-    <mergeCell ref="O37:O42"/>
+    <mergeCell ref="A85:A93"/>
+    <mergeCell ref="L80:L84"/>
+    <mergeCell ref="G80:G84"/>
+    <mergeCell ref="F80:F84"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="L85:L93"/>
+    <mergeCell ref="G85:G93"/>
+    <mergeCell ref="F85:F93"/>
+    <mergeCell ref="E85:E93"/>
+    <mergeCell ref="D85:D93"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="B85:B93"/>
+    <mergeCell ref="C85:C93"/>
+    <mergeCell ref="A71:A79"/>
+    <mergeCell ref="L68:L69"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="L71:L79"/>
+    <mergeCell ref="G71:G79"/>
+    <mergeCell ref="F71:F79"/>
+    <mergeCell ref="E71:E79"/>
+    <mergeCell ref="D71:D79"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B71:B79"/>
+    <mergeCell ref="C71:C79"/>
+    <mergeCell ref="G48:G56"/>
+    <mergeCell ref="F48:F56"/>
+    <mergeCell ref="E48:E56"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="G37:G42"/>
+    <mergeCell ref="L37:L42"/>
+    <mergeCell ref="D48:D56"/>
+    <mergeCell ref="A48:A56"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="L57:L61"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="E57:E61"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="L62:L67"/>
+    <mergeCell ref="G62:G67"/>
+    <mergeCell ref="F62:F67"/>
+    <mergeCell ref="E62:E67"/>
+    <mergeCell ref="D62:D67"/>
+    <mergeCell ref="L48:L56"/>
+    <mergeCell ref="B48:B56"/>
+    <mergeCell ref="D27:D34"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B27:B34"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="L27:L34"/>
+    <mergeCell ref="G27:G34"/>
+    <mergeCell ref="F27:F34"/>
+    <mergeCell ref="E27:E34"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="D2:D18"/>
+    <mergeCell ref="G2:G18"/>
+    <mergeCell ref="L2:L18"/>
+    <mergeCell ref="E2:E18"/>
+    <mergeCell ref="F2:F18"/>
+    <mergeCell ref="B2:B18"/>
+    <mergeCell ref="C2:C18"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="E37:E42"/>
+    <mergeCell ref="C48:C56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="C62:C67"/>
     <mergeCell ref="M80:M84"/>
     <mergeCell ref="M85:M93"/>
     <mergeCell ref="N2:N18"/>
@@ -4166,102 +4272,18 @@
     <mergeCell ref="M22:M24"/>
     <mergeCell ref="M27:M34"/>
     <mergeCell ref="M37:M42"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="E37:E42"/>
-    <mergeCell ref="C48:C56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="D2:D18"/>
-    <mergeCell ref="G2:G18"/>
-    <mergeCell ref="L2:L18"/>
-    <mergeCell ref="E2:E18"/>
-    <mergeCell ref="F2:F18"/>
-    <mergeCell ref="B2:B18"/>
-    <mergeCell ref="C2:C18"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D27:D34"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="B27:B34"/>
-    <mergeCell ref="C27:C34"/>
-    <mergeCell ref="L27:L34"/>
-    <mergeCell ref="G27:G34"/>
-    <mergeCell ref="F27:F34"/>
-    <mergeCell ref="E27:E34"/>
-    <mergeCell ref="G48:G56"/>
-    <mergeCell ref="F48:F56"/>
-    <mergeCell ref="E48:E56"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="G37:G42"/>
-    <mergeCell ref="L37:L42"/>
-    <mergeCell ref="D48:D56"/>
-    <mergeCell ref="A48:A56"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="L57:L61"/>
-    <mergeCell ref="G57:G61"/>
-    <mergeCell ref="F57:F61"/>
-    <mergeCell ref="E57:E61"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="L62:L67"/>
-    <mergeCell ref="G62:G67"/>
-    <mergeCell ref="F62:F67"/>
-    <mergeCell ref="E62:E67"/>
-    <mergeCell ref="D62:D67"/>
-    <mergeCell ref="L48:L56"/>
-    <mergeCell ref="B48:B56"/>
-    <mergeCell ref="A71:A79"/>
-    <mergeCell ref="L68:L69"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="L71:L79"/>
-    <mergeCell ref="G71:G79"/>
-    <mergeCell ref="F71:F79"/>
-    <mergeCell ref="E71:E79"/>
-    <mergeCell ref="D71:D79"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B71:B79"/>
-    <mergeCell ref="C71:C79"/>
-    <mergeCell ref="A85:A93"/>
-    <mergeCell ref="L80:L84"/>
-    <mergeCell ref="G80:G84"/>
-    <mergeCell ref="F80:F84"/>
-    <mergeCell ref="E80:E84"/>
-    <mergeCell ref="D80:D84"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="L85:L93"/>
-    <mergeCell ref="G85:G93"/>
-    <mergeCell ref="F85:F93"/>
-    <mergeCell ref="E85:E93"/>
-    <mergeCell ref="D85:D93"/>
-    <mergeCell ref="B80:B84"/>
-    <mergeCell ref="C80:C84"/>
-    <mergeCell ref="B85:B93"/>
-    <mergeCell ref="C85:C93"/>
+    <mergeCell ref="O80:O84"/>
+    <mergeCell ref="O85:O93"/>
+    <mergeCell ref="O48:O56"/>
+    <mergeCell ref="O57:O61"/>
+    <mergeCell ref="O62:O67"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="O71:O79"/>
+    <mergeCell ref="O2:O18"/>
+    <mergeCell ref="O19:O21"/>
+    <mergeCell ref="O22:O24"/>
+    <mergeCell ref="O27:O34"/>
+    <mergeCell ref="O37:O42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Name change of hus_blt_yr
</commit_message>
<xml_diff>
--- a/data/log_data_postprocess.xlsx
+++ b/data/log_data_postprocess.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProject\EDA-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6C570A-5581-4994-A498-01BAC8AB140D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F8AE5F-7A99-4376-BE51-AF3196574C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B16BB66F-007C-416B-8A77-4B4F8B6782B4}"/>
   </bookViews>
@@ -584,9 +584,6 @@
     <t>after 2010</t>
   </si>
   <si>
-    <t>cat_hus_blt_yr</t>
-  </si>
-  <si>
     <t>Banded house blt year</t>
   </si>
   <si>
@@ -624,9 +621,6 @@
   </si>
   <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>No Need to Modify</t>
   </si>
   <si>
     <t>Not in 2017, 2016. Will not be used in sKor data.</t>
@@ -992,6 +986,34 @@
   </si>
   <si>
     <t>age:60-64 → 67</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cat_hus_blt_yr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+num_hus_blt_yr</t>
+    </r>
+  </si>
+  <si>
+    <t>No Need to Modify
+→ Change type into numerical!</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1239,86 +1261,92 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1638,8 +1666,8 @@
   <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D18"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L37" sqref="L37:L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,35 +1725,35 @@
         <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="23">
         <v>3</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="23" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="5">
@@ -1740,27 +1768,27 @@
       <c r="K2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="M2" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>192</v>
+      <c r="M2" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="N2" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="O2" s="47" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="3">
         <v>21</v>
       </c>
@@ -1773,19 +1801,19 @@
       <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="3">
         <v>22</v>
       </c>
@@ -1798,19 +1826,19 @@
       <c r="K4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="35"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="5">
         <v>23</v>
       </c>
@@ -1823,19 +1851,19 @@
       <c r="K5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="35"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="3">
         <v>24</v>
       </c>
@@ -1848,19 +1876,19 @@
       <c r="K6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="35"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="6">
         <v>25</v>
       </c>
@@ -1873,19 +1901,19 @@
       <c r="K7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="35"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="3">
         <v>26</v>
       </c>
@@ -1898,19 +1926,19 @@
       <c r="K8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="6">
         <v>29</v>
       </c>
@@ -1923,19 +1951,19 @@
       <c r="K9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="33"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="5">
         <v>31</v>
       </c>
@@ -1948,19 +1976,19 @@
       <c r="K10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="5">
         <v>32</v>
       </c>
@@ -1973,19 +2001,19 @@
       <c r="K11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="35"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="6">
         <v>33</v>
       </c>
@@ -1998,19 +2026,19 @@
       <c r="K12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="35"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="6">
         <v>34</v>
       </c>
@@ -2023,19 +2051,19 @@
       <c r="K13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="35"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="3">
         <v>35</v>
       </c>
@@ -2048,19 +2076,19 @@
       <c r="K14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="3">
         <v>36</v>
       </c>
@@ -2073,19 +2101,19 @@
       <c r="K15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="35"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="6">
         <v>37</v>
       </c>
@@ -2098,19 +2126,19 @@
       <c r="K16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="35"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="33"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="3">
         <v>38</v>
       </c>
@@ -2123,19 +2151,19 @@
       <c r="K17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="33"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="3">
         <v>39</v>
       </c>
@@ -2148,31 +2176,31 @@
       <c r="K18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="35"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="26">
         <v>2</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="26" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="4">
@@ -2187,27 +2215,27 @@
       <c r="K19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L19" s="39" t="s">
+      <c r="L19" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="M19" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="N19" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="O19" s="22" t="s">
-        <v>192</v>
+      <c r="M19" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="N19" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="O19" s="44" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
       <c r="H20" s="4">
         <v>2</v>
       </c>
@@ -2220,19 +2248,19 @@
       <c r="K20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L20" s="40"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
       <c r="H21" s="4">
         <v>3</v>
       </c>
@@ -2245,31 +2273,31 @@
       <c r="K21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="40"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" s="25" t="s">
+      <c r="C22" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="23">
         <v>3</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="23" t="s">
         <v>41</v>
       </c>
       <c r="H22" s="3">
@@ -2280,27 +2308,27 @@
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="N22" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="O22" s="25" t="s">
-        <v>192</v>
+      <c r="L22" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="M22" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="N22" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="O22" s="23" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
       <c r="H23" s="3">
         <v>2</v>
       </c>
@@ -2309,19 +2337,19 @@
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="3">
         <v>3</v>
       </c>
@@ -2330,10 +2358,10 @@
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -2343,7 +2371,7 @@
         <v>161</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>49</v>
@@ -2360,16 +2388,16 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2380,7 +2408,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>50</v>
@@ -2397,38 +2425,38 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="26">
         <v>4</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H27" s="11">
@@ -2443,27 +2471,27 @@
       <c r="K27" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="L27" s="39" t="s">
+      <c r="L27" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="M27" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="N27" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="O27" s="22" t="s">
-        <v>192</v>
+      <c r="M27" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="N27" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="O27" s="44" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="11">
         <v>2</v>
       </c>
@@ -2476,19 +2504,19 @@
       <c r="K28" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L28" s="40"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
       <c r="H29" s="4">
         <v>3</v>
       </c>
@@ -2501,19 +2529,19 @@
       <c r="K29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="L29" s="40"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="5">
         <v>4</v>
       </c>
@@ -2526,19 +2554,19 @@
       <c r="K30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L30" s="40"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="6">
         <v>5</v>
       </c>
@@ -2551,19 +2579,19 @@
       <c r="K31" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="L31" s="40"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
       <c r="H32" s="6">
         <v>6</v>
       </c>
@@ -2576,19 +2604,19 @@
       <c r="K32" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L32" s="40"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
       <c r="H33" s="5">
         <v>7</v>
       </c>
@@ -2601,19 +2629,19 @@
       <c r="K33" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="L33" s="40"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
       <c r="H34" s="5">
         <v>8</v>
       </c>
@@ -2626,17 +2654,17 @@
       <c r="K34" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L34" s="40"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12" t="s">
@@ -2654,7 +2682,7 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
@@ -2679,33 +2707,31 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
       <c r="O36" s="18"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30" t="s">
         <v>179</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F37" s="27">
-        <v>6</v>
-      </c>
-      <c r="G37" s="27" t="s">
-        <v>180</v>
       </c>
       <c r="H37" s="8">
         <v>1</v>
@@ -2715,27 +2741,27 @@
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
-      <c r="L37" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="M37" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="N37" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="O37" s="27" t="s">
-        <v>192</v>
+      <c r="L37" s="50" t="s">
+        <v>239</v>
+      </c>
+      <c r="M37" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N37" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="O37" s="30" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
       <c r="H38" s="8">
         <v>2</v>
       </c>
@@ -2744,19 +2770,19 @@
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="28"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
       <c r="H39" s="8">
         <v>3</v>
       </c>
@@ -2765,19 +2791,19 @@
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
-      <c r="L39" s="42"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
-      <c r="O39" s="28"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
       <c r="H40" s="8">
         <v>4</v>
       </c>
@@ -2786,19 +2812,19 @@
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
       <c r="H41" s="8">
         <v>5</v>
       </c>
@@ -2807,19 +2833,19 @@
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="28"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
       <c r="H42" s="8">
         <v>6</v>
       </c>
@@ -2828,10 +2854,10 @@
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
-      <c r="L42" s="43"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="32"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -2843,7 +2869,7 @@
       <c r="C43" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="22" t="s">
         <v>71</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -2858,16 +2884,16 @@
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O43" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -2895,16 +2921,16 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O44" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -2932,16 +2958,16 @@
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
       <c r="L45" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M45" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N45" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O45" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -2969,16 +2995,16 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O46" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -2989,7 +3015,7 @@
         <v>171</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>83</v>
@@ -3009,33 +3035,33 @@
         <v>85</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N47" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O47" s="7"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="C48" s="27" t="s">
-        <v>203</v>
-      </c>
-      <c r="D48" s="23" t="s">
+      <c r="B48" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="D48" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="23" t="s">
+      <c r="E48" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F48" s="26">
         <v>5</v>
       </c>
-      <c r="G48" s="23" t="s">
+      <c r="G48" s="26" t="s">
         <v>88</v>
       </c>
       <c r="H48" s="11">
@@ -3050,27 +3076,27 @@
       <c r="K48" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L48" s="39" t="s">
+      <c r="L48" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="M48" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="N48" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="O48" s="22" t="s">
-        <v>192</v>
+      <c r="M48" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="N48" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="O48" s="44" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
       <c r="H49" s="10">
         <v>2</v>
       </c>
@@ -3083,19 +3109,19 @@
       <c r="K49" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L49" s="40"/>
-      <c r="M49" s="23"/>
-      <c r="N49" s="23"/>
-      <c r="O49" s="23"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
       <c r="H50" s="10">
         <v>3</v>
       </c>
@@ -3108,19 +3134,19 @@
       <c r="K50" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="L50" s="40"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="23"/>
-      <c r="O50" s="23"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="26"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
       <c r="H51" s="9">
         <v>4</v>
       </c>
@@ -3133,19 +3159,19 @@
       <c r="K51" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="L51" s="40"/>
-      <c r="M51" s="23"/>
-      <c r="N51" s="23"/>
-      <c r="O51" s="23"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
       <c r="H52" s="9">
         <v>5</v>
       </c>
@@ -3158,19 +3184,19 @@
       <c r="K52" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L52" s="40"/>
-      <c r="M52" s="23"/>
-      <c r="N52" s="23"/>
-      <c r="O52" s="23"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
       <c r="H53" s="4">
         <v>6</v>
       </c>
@@ -3183,19 +3209,19 @@
       <c r="K53" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="L53" s="40"/>
-      <c r="M53" s="23"/>
-      <c r="N53" s="23"/>
-      <c r="O53" s="23"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="26"/>
+      <c r="N53" s="26"/>
+      <c r="O53" s="26"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
       <c r="H54" s="5">
         <v>7</v>
       </c>
@@ -3208,19 +3234,19 @@
       <c r="K54" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L54" s="40"/>
-      <c r="M54" s="23"/>
-      <c r="N54" s="23"/>
-      <c r="O54" s="23"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
       <c r="H55" s="5">
         <v>8</v>
       </c>
@@ -3233,19 +3259,19 @@
       <c r="K55" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="L55" s="40"/>
-      <c r="M55" s="23"/>
-      <c r="N55" s="23"/>
-      <c r="O55" s="23"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="26"/>
+      <c r="N55" s="26"/>
+      <c r="O55" s="26"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
       <c r="H56" s="11">
         <v>9</v>
       </c>
@@ -3258,31 +3284,31 @@
       <c r="K56" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="L56" s="40"/>
-      <c r="M56" s="23"/>
-      <c r="N56" s="23"/>
-      <c r="O56" s="23"/>
+      <c r="L56" s="25"/>
+      <c r="M56" s="26"/>
+      <c r="N56" s="26"/>
+      <c r="O56" s="26"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
+      <c r="A57" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="D57" s="25" t="s">
+      <c r="B57" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="D57" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F57" s="25">
+      <c r="F57" s="23">
         <v>3</v>
       </c>
-      <c r="G57" s="25" t="s">
+      <c r="G57" s="23" t="s">
         <v>100</v>
       </c>
       <c r="H57" s="3">
@@ -3293,27 +3319,27 @@
       </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
-      <c r="L57" s="34" t="s">
-        <v>214</v>
-      </c>
-      <c r="M57" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="N57" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="O57" s="24" t="s">
-        <v>192</v>
+      <c r="L57" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="M57" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="N57" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="O57" s="47" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
       <c r="H58" s="3">
         <v>2</v>
       </c>
@@ -3322,19 +3348,19 @@
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="25"/>
-      <c r="N58" s="25"/>
-      <c r="O58" s="25"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="23"/>
+      <c r="N58" s="23"/>
+      <c r="O58" s="23"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
       <c r="H59" s="3">
         <v>3</v>
       </c>
@@ -3343,19 +3369,19 @@
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="25"/>
-      <c r="N59" s="25"/>
-      <c r="O59" s="25"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="23"/>
+      <c r="N59" s="23"/>
+      <c r="O59" s="23"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
       <c r="H60" s="21">
         <v>4</v>
       </c>
@@ -3364,19 +3390,19 @@
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="25"/>
-      <c r="O60" s="25"/>
+      <c r="L60" s="28"/>
+      <c r="M60" s="23"/>
+      <c r="N60" s="23"/>
+      <c r="O60" s="23"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
       <c r="H61" s="21">
         <v>5</v>
       </c>
@@ -3385,31 +3411,31 @@
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="25"/>
-      <c r="N61" s="25"/>
-      <c r="O61" s="25"/>
+      <c r="L61" s="28"/>
+      <c r="M61" s="23"/>
+      <c r="N61" s="23"/>
+      <c r="O61" s="23"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
+      <c r="A62" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="C62" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="D62" s="23" t="s">
+      <c r="B62" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="D62" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="E62" s="23" t="s">
+      <c r="E62" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F62" s="23">
+      <c r="F62" s="26">
         <v>3</v>
       </c>
-      <c r="G62" s="23" t="s">
+      <c r="G62" s="26" t="s">
         <v>108</v>
       </c>
       <c r="H62" s="21">
@@ -3420,27 +3446,27 @@
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="M62" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="N62" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="O62" s="22" t="s">
-        <v>192</v>
+      <c r="L62" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="M62" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="N62" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="O62" s="44" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
       <c r="H63" s="21">
         <v>2</v>
       </c>
@@ -3449,19 +3475,19 @@
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
-      <c r="L63" s="40"/>
-      <c r="M63" s="23"/>
-      <c r="N63" s="23"/>
-      <c r="O63" s="23"/>
+      <c r="L63" s="25"/>
+      <c r="M63" s="26"/>
+      <c r="N63" s="26"/>
+      <c r="O63" s="26"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="28"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
       <c r="H64" s="4">
         <v>3</v>
       </c>
@@ -3470,19 +3496,19 @@
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="40"/>
-      <c r="M64" s="23"/>
-      <c r="N64" s="23"/>
-      <c r="O64" s="23"/>
+      <c r="L64" s="25"/>
+      <c r="M64" s="26"/>
+      <c r="N64" s="26"/>
+      <c r="O64" s="26"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="28"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="23"/>
+      <c r="A65" s="26"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
       <c r="H65" s="4">
         <v>4</v>
       </c>
@@ -3491,19 +3517,19 @@
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
-      <c r="L65" s="40"/>
-      <c r="M65" s="23"/>
-      <c r="N65" s="23"/>
-      <c r="O65" s="23"/>
+      <c r="L65" s="25"/>
+      <c r="M65" s="26"/>
+      <c r="N65" s="26"/>
+      <c r="O65" s="26"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26"/>
       <c r="H66" s="4">
         <v>5</v>
       </c>
@@ -3512,19 +3538,19 @@
       </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
-      <c r="L66" s="40"/>
-      <c r="M66" s="23"/>
-      <c r="N66" s="23"/>
-      <c r="O66" s="23"/>
+      <c r="L66" s="25"/>
+      <c r="M66" s="26"/>
+      <c r="N66" s="26"/>
+      <c r="O66" s="26"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-      <c r="B67" s="29"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
       <c r="H67" s="21">
         <v>6</v>
       </c>
@@ -3533,31 +3559,31 @@
       </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="40"/>
-      <c r="M67" s="23"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="23"/>
+      <c r="L67" s="25"/>
+      <c r="M67" s="26"/>
+      <c r="N67" s="26"/>
+      <c r="O67" s="26"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="45" t="s">
+      <c r="A68" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B68" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="C68" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="D68" s="45" t="s">
+      <c r="B68" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="C68" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="D68" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="E68" s="45" t="s">
+      <c r="E68" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="F68" s="45">
+      <c r="F68" s="35">
         <v>2</v>
       </c>
-      <c r="G68" s="45" t="s">
+      <c r="G68" s="35" t="s">
         <v>115</v>
       </c>
       <c r="H68" s="21">
@@ -3568,21 +3594,21 @@
       </c>
       <c r="J68" s="16"/>
       <c r="K68" s="16"/>
-      <c r="L68" s="44" t="s">
-        <v>195</v>
-      </c>
-      <c r="M68" s="26"/>
-      <c r="N68" s="26"/>
-      <c r="O68" s="26"/>
+      <c r="L68" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="M68" s="48"/>
+      <c r="N68" s="48"/>
+      <c r="O68" s="48"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="46"/>
-      <c r="B69" s="46"/>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46"/>
-      <c r="G69" s="46"/>
+      <c r="A69" s="36"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
       <c r="H69" s="21">
         <v>2</v>
       </c>
@@ -3591,20 +3617,20 @@
       </c>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
-      <c r="L69" s="44"/>
-      <c r="M69" s="26"/>
-      <c r="N69" s="26"/>
-      <c r="O69" s="26"/>
+      <c r="L69" s="34"/>
+      <c r="M69" s="48"/>
+      <c r="N69" s="48"/>
+      <c r="O69" s="48"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>117</v>
@@ -3621,16 +3647,16 @@
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M70" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N70" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O70" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
@@ -3638,28 +3664,28 @@
         <v>119</v>
       </c>
       <c r="B71" s="33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="D71" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="E71" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="D71" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="E71" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F71" s="25">
+      <c r="F71" s="23">
         <v>3</v>
       </c>
-      <c r="G71" s="25" t="s">
+      <c r="G71" s="23" t="s">
         <v>120</v>
       </c>
       <c r="H71" s="3">
         <v>1</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J71" s="21">
         <v>1</v>
@@ -3667,32 +3693,32 @@
       <c r="K71" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="L71" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="M71" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="N71" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="O71" s="24" t="s">
-        <v>192</v>
+      <c r="L71" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="M71" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="N71" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="O71" s="47" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="33"/>
       <c r="B72" s="33"/>
       <c r="C72" s="33"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
       <c r="H72" s="3">
         <v>2</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J72" s="21">
         <v>1</v>
@@ -3700,24 +3726,24 @@
       <c r="K72" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="L72" s="35"/>
-      <c r="M72" s="25"/>
-      <c r="N72" s="25"/>
-      <c r="O72" s="25"/>
+      <c r="L72" s="28"/>
+      <c r="M72" s="23"/>
+      <c r="N72" s="23"/>
+      <c r="O72" s="23"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="33"/>
       <c r="B73" s="33"/>
       <c r="C73" s="33"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
       <c r="H73" s="3">
         <v>3</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J73" s="21">
         <v>1</v>
@@ -3725,24 +3751,24 @@
       <c r="K73" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="L73" s="35"/>
-      <c r="M73" s="25"/>
-      <c r="N73" s="25"/>
-      <c r="O73" s="25"/>
+      <c r="L73" s="28"/>
+      <c r="M73" s="23"/>
+      <c r="N73" s="23"/>
+      <c r="O73" s="23"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="33"/>
       <c r="B74" s="33"/>
       <c r="C74" s="33"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
       <c r="H74" s="3">
         <v>4</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J74" s="21">
         <v>2</v>
@@ -3750,24 +3776,24 @@
       <c r="K74" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="L74" s="35"/>
-      <c r="M74" s="25"/>
-      <c r="N74" s="25"/>
-      <c r="O74" s="25"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="23"/>
+      <c r="N74" s="23"/>
+      <c r="O74" s="23"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="33"/>
       <c r="B75" s="33"/>
       <c r="C75" s="33"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="25"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
       <c r="H75" s="3">
         <v>5</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J75" s="21">
         <v>2</v>
@@ -3775,24 +3801,24 @@
       <c r="K75" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="L75" s="35"/>
-      <c r="M75" s="25"/>
-      <c r="N75" s="25"/>
-      <c r="O75" s="25"/>
+      <c r="L75" s="28"/>
+      <c r="M75" s="23"/>
+      <c r="N75" s="23"/>
+      <c r="O75" s="23"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="33"/>
       <c r="B76" s="33"/>
       <c r="C76" s="33"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
       <c r="H76" s="3">
         <v>6</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J76" s="21">
         <v>2</v>
@@ -3800,24 +3826,24 @@
       <c r="K76" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="L76" s="35"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="25"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="23"/>
+      <c r="N76" s="23"/>
+      <c r="O76" s="23"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="33"/>
       <c r="B77" s="33"/>
       <c r="C77" s="33"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
       <c r="H77" s="3">
         <v>7</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J77" s="21">
         <v>2</v>
@@ -3825,24 +3851,24 @@
       <c r="K77" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="L77" s="35"/>
-      <c r="M77" s="25"/>
-      <c r="N77" s="25"/>
-      <c r="O77" s="25"/>
+      <c r="L77" s="28"/>
+      <c r="M77" s="23"/>
+      <c r="N77" s="23"/>
+      <c r="O77" s="23"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="33"/>
       <c r="B78" s="33"/>
       <c r="C78" s="33"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
       <c r="H78" s="3">
         <v>8</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J78" s="21">
         <v>3</v>
@@ -3850,24 +3876,24 @@
       <c r="K78" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="L78" s="35"/>
-      <c r="M78" s="25"/>
-      <c r="N78" s="25"/>
-      <c r="O78" s="25"/>
+      <c r="L78" s="28"/>
+      <c r="M78" s="23"/>
+      <c r="N78" s="23"/>
+      <c r="O78" s="23"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="33"/>
       <c r="B79" s="33"/>
       <c r="C79" s="33"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
       <c r="H79" s="3">
         <v>9</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J79" s="21">
         <v>3</v>
@@ -3875,31 +3901,31 @@
       <c r="K79" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="L79" s="35"/>
-      <c r="M79" s="25"/>
-      <c r="N79" s="25"/>
-      <c r="O79" s="25"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="23"/>
+      <c r="N79" s="23"/>
+      <c r="O79" s="23"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A80" s="23" t="s">
+      <c r="A80" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B80" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="C80" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="D80" s="23" t="s">
+      <c r="B80" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="D80" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="E80" s="23" t="s">
+      <c r="E80" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F80" s="23">
+      <c r="F80" s="26">
         <v>4</v>
       </c>
-      <c r="G80" s="23" t="s">
+      <c r="G80" s="26" t="s">
         <v>132</v>
       </c>
       <c r="H80" s="4">
@@ -3910,27 +3936,27 @@
       </c>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
-      <c r="L80" s="39" t="s">
+      <c r="L80" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="M80" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="N80" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="O80" s="22" t="s">
-        <v>192</v>
+      <c r="M80" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="N80" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="O80" s="44" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
       <c r="H81" s="4">
         <v>2</v>
       </c>
@@ -3939,19 +3965,19 @@
       </c>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
-      <c r="L81" s="40"/>
-      <c r="M81" s="23"/>
-      <c r="N81" s="23"/>
-      <c r="O81" s="23"/>
+      <c r="L81" s="25"/>
+      <c r="M81" s="26"/>
+      <c r="N81" s="26"/>
+      <c r="O81" s="26"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
-      <c r="B82" s="23"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="23"/>
+      <c r="A82" s="26"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="26"/>
       <c r="H82" s="4">
         <v>3</v>
       </c>
@@ -3960,19 +3986,19 @@
       </c>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
-      <c r="L82" s="40"/>
-      <c r="M82" s="23"/>
-      <c r="N82" s="23"/>
-      <c r="O82" s="23"/>
+      <c r="L82" s="25"/>
+      <c r="M82" s="26"/>
+      <c r="N82" s="26"/>
+      <c r="O82" s="26"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" s="23"/>
-      <c r="B83" s="23"/>
-      <c r="C83" s="23"/>
-      <c r="D83" s="23"/>
-      <c r="E83" s="23"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="23"/>
+      <c r="A83" s="26"/>
+      <c r="B83" s="26"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="26"/>
+      <c r="G83" s="26"/>
       <c r="H83" s="4">
         <v>4</v>
       </c>
@@ -3981,19 +4007,19 @@
       </c>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
-      <c r="L83" s="40"/>
-      <c r="M83" s="23"/>
-      <c r="N83" s="23"/>
-      <c r="O83" s="23"/>
+      <c r="L83" s="25"/>
+      <c r="M83" s="26"/>
+      <c r="N83" s="26"/>
+      <c r="O83" s="26"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" s="23"/>
-      <c r="B84" s="23"/>
-      <c r="C84" s="23"/>
-      <c r="D84" s="23"/>
-      <c r="E84" s="23"/>
-      <c r="F84" s="23"/>
-      <c r="G84" s="23"/>
+      <c r="A84" s="26"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="26"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="26"/>
+      <c r="G84" s="26"/>
       <c r="H84" s="4">
         <v>5</v>
       </c>
@@ -4002,38 +4028,38 @@
       </c>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
-      <c r="L84" s="40"/>
-      <c r="M84" s="23"/>
-      <c r="N84" s="23"/>
-      <c r="O84" s="23"/>
+      <c r="L84" s="25"/>
+      <c r="M84" s="26"/>
+      <c r="N84" s="26"/>
+      <c r="O84" s="26"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A85" s="25" t="s">
+      <c r="A85" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="B85" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="C85" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="D85" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="E85" s="25" t="s">
+      <c r="B85" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D85" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="E85" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F85" s="25">
+      <c r="F85" s="23">
         <v>7</v>
       </c>
-      <c r="G85" s="25" t="s">
+      <c r="G85" s="23" t="s">
         <v>138</v>
       </c>
       <c r="H85" s="3">
         <v>1</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J85" s="21">
         <v>1</v>
@@ -4041,32 +4067,32 @@
       <c r="K85" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="L85" s="34" t="s">
-        <v>235</v>
-      </c>
-      <c r="M85" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="N85" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="O85" s="24" t="s">
-        <v>192</v>
+      <c r="L85" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="M85" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="N85" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="O85" s="47" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" s="25"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="25"/>
+      <c r="A86" s="23"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
       <c r="H86" s="3">
         <v>2</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J86" s="21">
         <v>2</v>
@@ -4074,24 +4100,24 @@
       <c r="K86" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="L86" s="35"/>
-      <c r="M86" s="25"/>
-      <c r="N86" s="25"/>
-      <c r="O86" s="25"/>
+      <c r="L86" s="28"/>
+      <c r="M86" s="23"/>
+      <c r="N86" s="23"/>
+      <c r="O86" s="23"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
-      <c r="G87" s="25"/>
+      <c r="A87" s="23"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
       <c r="H87" s="3">
         <v>3</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J87" s="21">
         <v>3</v>
@@ -4099,24 +4125,24 @@
       <c r="K87" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="L87" s="35"/>
-      <c r="M87" s="25"/>
-      <c r="N87" s="25"/>
-      <c r="O87" s="25"/>
+      <c r="L87" s="28"/>
+      <c r="M87" s="23"/>
+      <c r="N87" s="23"/>
+      <c r="O87" s="23"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="25"/>
+      <c r="A88" s="23"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
       <c r="H88" s="3">
         <v>4</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J88" s="21">
         <v>4</v>
@@ -4124,24 +4150,24 @@
       <c r="K88" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="L88" s="35"/>
-      <c r="M88" s="25"/>
-      <c r="N88" s="25"/>
-      <c r="O88" s="25"/>
+      <c r="L88" s="28"/>
+      <c r="M88" s="23"/>
+      <c r="N88" s="23"/>
+      <c r="O88" s="23"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="25"/>
+      <c r="A89" s="23"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
       <c r="H89" s="3">
         <v>5</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J89" s="21">
         <v>5</v>
@@ -4149,24 +4175,24 @@
       <c r="K89" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="L89" s="35"/>
-      <c r="M89" s="25"/>
-      <c r="N89" s="25"/>
-      <c r="O89" s="25"/>
+      <c r="L89" s="28"/>
+      <c r="M89" s="23"/>
+      <c r="N89" s="23"/>
+      <c r="O89" s="23"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="25"/>
+      <c r="A90" s="23"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
       <c r="H90" s="3">
         <v>6</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J90" s="21">
         <v>6</v>
@@ -4174,24 +4200,24 @@
       <c r="K90" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="L90" s="35"/>
-      <c r="M90" s="25"/>
-      <c r="N90" s="25"/>
-      <c r="O90" s="25"/>
+      <c r="L90" s="28"/>
+      <c r="M90" s="23"/>
+      <c r="N90" s="23"/>
+      <c r="O90" s="23"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="25"/>
+      <c r="A91" s="23"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
       <c r="H91" s="3">
         <v>7</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J91" s="21">
         <v>7</v>
@@ -4199,24 +4225,24 @@
       <c r="K91" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="L91" s="35"/>
-      <c r="M91" s="25"/>
-      <c r="N91" s="25"/>
-      <c r="O91" s="25"/>
+      <c r="L91" s="28"/>
+      <c r="M91" s="23"/>
+      <c r="N91" s="23"/>
+      <c r="O91" s="23"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A92" s="25"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="25"/>
+      <c r="A92" s="23"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
       <c r="H92" s="3">
         <v>8</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J92" s="21">
         <v>7</v>
@@ -4224,24 +4250,24 @@
       <c r="K92" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="L92" s="35"/>
-      <c r="M92" s="25"/>
-      <c r="N92" s="25"/>
-      <c r="O92" s="25"/>
+      <c r="L92" s="28"/>
+      <c r="M92" s="23"/>
+      <c r="N92" s="23"/>
+      <c r="O92" s="23"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
-      <c r="G93" s="25"/>
+      <c r="A93" s="23"/>
+      <c r="B93" s="23"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="23"/>
+      <c r="G93" s="23"/>
       <c r="H93" s="3">
         <v>9</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J93" s="21">
         <v>7</v>
@@ -4249,20 +4275,20 @@
       <c r="K93" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="L93" s="35"/>
-      <c r="M93" s="25"/>
-      <c r="N93" s="25"/>
-      <c r="O93" s="25"/>
+      <c r="L93" s="28"/>
+      <c r="M93" s="23"/>
+      <c r="N93" s="23"/>
+      <c r="O93" s="23"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>148</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>149</v>
@@ -4282,34 +4308,110 @@
         <v>151</v>
       </c>
       <c r="M94" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N94" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O94" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:O94" xr:uid="{1BA5C2C4-4AF8-44A6-8680-53141E329A99}"/>
   <mergeCells count="132">
-    <mergeCell ref="A85:A93"/>
-    <mergeCell ref="L80:L84"/>
-    <mergeCell ref="G80:G84"/>
-    <mergeCell ref="F80:F84"/>
-    <mergeCell ref="E80:E84"/>
-    <mergeCell ref="D80:D84"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="L85:L93"/>
-    <mergeCell ref="G85:G93"/>
-    <mergeCell ref="F85:F93"/>
-    <mergeCell ref="E85:E93"/>
-    <mergeCell ref="D85:D93"/>
-    <mergeCell ref="B80:B84"/>
-    <mergeCell ref="C80:C84"/>
-    <mergeCell ref="B85:B93"/>
-    <mergeCell ref="C85:C93"/>
+    <mergeCell ref="O80:O84"/>
+    <mergeCell ref="O85:O93"/>
+    <mergeCell ref="O48:O56"/>
+    <mergeCell ref="O57:O61"/>
+    <mergeCell ref="O62:O67"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="O71:O79"/>
+    <mergeCell ref="O2:O18"/>
+    <mergeCell ref="O19:O21"/>
+    <mergeCell ref="O22:O24"/>
+    <mergeCell ref="O27:O34"/>
+    <mergeCell ref="O37:O42"/>
+    <mergeCell ref="M85:M93"/>
+    <mergeCell ref="N2:N18"/>
+    <mergeCell ref="N19:N21"/>
+    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="N27:N34"/>
+    <mergeCell ref="N37:N42"/>
+    <mergeCell ref="N48:N56"/>
+    <mergeCell ref="N57:N61"/>
+    <mergeCell ref="N62:N67"/>
+    <mergeCell ref="N68:N69"/>
+    <mergeCell ref="N71:N79"/>
+    <mergeCell ref="N80:N84"/>
+    <mergeCell ref="N85:N93"/>
+    <mergeCell ref="M48:M56"/>
+    <mergeCell ref="M57:M61"/>
+    <mergeCell ref="M62:M67"/>
+    <mergeCell ref="M68:M69"/>
+    <mergeCell ref="M71:M79"/>
+    <mergeCell ref="M2:M18"/>
+    <mergeCell ref="M19:M21"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="M27:M34"/>
+    <mergeCell ref="M37:M42"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="E37:E42"/>
+    <mergeCell ref="C48:C56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="M80:M84"/>
+    <mergeCell ref="G48:G56"/>
+    <mergeCell ref="F48:F56"/>
+    <mergeCell ref="E48:E56"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="G37:G42"/>
+    <mergeCell ref="L37:L42"/>
+    <mergeCell ref="D48:D56"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="D2:D18"/>
+    <mergeCell ref="G2:G18"/>
+    <mergeCell ref="L2:L18"/>
+    <mergeCell ref="E2:E18"/>
+    <mergeCell ref="F2:F18"/>
+    <mergeCell ref="B2:B18"/>
+    <mergeCell ref="C2:C18"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D27:D34"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B27:B34"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="L27:L34"/>
+    <mergeCell ref="G27:G34"/>
+    <mergeCell ref="F27:F34"/>
+    <mergeCell ref="E27:E34"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="L62:L67"/>
+    <mergeCell ref="G62:G67"/>
+    <mergeCell ref="F62:F67"/>
+    <mergeCell ref="E62:E67"/>
+    <mergeCell ref="D62:D67"/>
+    <mergeCell ref="L48:L56"/>
+    <mergeCell ref="B48:B56"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="B37:B42"/>
     <mergeCell ref="A71:A79"/>
@@ -4334,98 +4436,22 @@
     <mergeCell ref="G57:G61"/>
     <mergeCell ref="F57:F61"/>
     <mergeCell ref="E57:E61"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="L62:L67"/>
-    <mergeCell ref="G62:G67"/>
-    <mergeCell ref="F62:F67"/>
-    <mergeCell ref="E62:E67"/>
-    <mergeCell ref="D62:D67"/>
-    <mergeCell ref="L48:L56"/>
-    <mergeCell ref="B48:B56"/>
-    <mergeCell ref="D27:D34"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="B27:B34"/>
-    <mergeCell ref="C27:C34"/>
-    <mergeCell ref="L27:L34"/>
-    <mergeCell ref="G27:G34"/>
-    <mergeCell ref="F27:F34"/>
-    <mergeCell ref="E27:E34"/>
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="D2:D18"/>
-    <mergeCell ref="G2:G18"/>
-    <mergeCell ref="L2:L18"/>
-    <mergeCell ref="E2:E18"/>
-    <mergeCell ref="F2:F18"/>
-    <mergeCell ref="B2:B18"/>
-    <mergeCell ref="C2:C18"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="E37:E42"/>
-    <mergeCell ref="C48:C56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="M80:M84"/>
-    <mergeCell ref="G48:G56"/>
-    <mergeCell ref="F48:F56"/>
-    <mergeCell ref="E48:E56"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="G37:G42"/>
-    <mergeCell ref="L37:L42"/>
-    <mergeCell ref="D48:D56"/>
-    <mergeCell ref="M85:M93"/>
-    <mergeCell ref="N2:N18"/>
-    <mergeCell ref="N19:N21"/>
-    <mergeCell ref="N22:N24"/>
-    <mergeCell ref="N27:N34"/>
-    <mergeCell ref="N37:N42"/>
-    <mergeCell ref="N48:N56"/>
-    <mergeCell ref="N57:N61"/>
-    <mergeCell ref="N62:N67"/>
-    <mergeCell ref="N68:N69"/>
-    <mergeCell ref="N71:N79"/>
-    <mergeCell ref="N80:N84"/>
-    <mergeCell ref="N85:N93"/>
-    <mergeCell ref="M48:M56"/>
-    <mergeCell ref="M57:M61"/>
-    <mergeCell ref="M62:M67"/>
-    <mergeCell ref="M68:M69"/>
-    <mergeCell ref="M71:M79"/>
-    <mergeCell ref="M2:M18"/>
-    <mergeCell ref="M19:M21"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="M27:M34"/>
-    <mergeCell ref="M37:M42"/>
-    <mergeCell ref="O80:O84"/>
-    <mergeCell ref="O85:O93"/>
-    <mergeCell ref="O48:O56"/>
-    <mergeCell ref="O57:O61"/>
-    <mergeCell ref="O62:O67"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="O71:O79"/>
-    <mergeCell ref="O2:O18"/>
-    <mergeCell ref="O19:O21"/>
-    <mergeCell ref="O22:O24"/>
-    <mergeCell ref="O27:O34"/>
-    <mergeCell ref="O37:O42"/>
+    <mergeCell ref="A85:A93"/>
+    <mergeCell ref="L80:L84"/>
+    <mergeCell ref="G80:G84"/>
+    <mergeCell ref="F80:F84"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="L85:L93"/>
+    <mergeCell ref="G85:G93"/>
+    <mergeCell ref="F85:F93"/>
+    <mergeCell ref="E85:E93"/>
+    <mergeCell ref="D85:D93"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="B85:B93"/>
+    <mergeCell ref="C85:C93"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>